<commit_message>
adding a while loop
</commit_message>
<xml_diff>
--- a/InputInvoice.xlsx
+++ b/InputInvoice.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1815" yWindow="45" windowWidth="20025" windowHeight="15480" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="工作表1" sheetId="1" state="visible" r:id="rId1"/>
@@ -504,10 +504,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F2" sqref="F2:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -557,11 +557,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
@@ -585,11 +585,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
@@ -613,11 +613,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
@@ -636,16 +636,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>T006.407.16.053.00</t>
+          <t>T094.210.11.111.00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2832</v>
+        <v>1652</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
@@ -664,16 +664,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>T094.210.11.111.00</t>
+          <t>T099.407.11.048.00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
@@ -681,7 +681,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1652</v>
+        <v>3953</v>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
@@ -692,16 +692,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>T099.407.11.048.00</t>
+          <t>T116.617.11.057.01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C7" s="3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3953</v>
+        <v>1888</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
@@ -720,12 +720,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>T116.617.11.057.01</t>
+          <t>T120.417.11.041.01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C8" s="3" t="n">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1888</v>
+        <v>2743.5</v>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
@@ -748,12 +748,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>T120.417.11.041.01</t>
+          <t>T120.417.11.091.01</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C9" s="3" t="n">
@@ -776,12 +776,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>T120.417.11.091.01</t>
+          <t>T126.010.11.013.00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C10" s="3" t="n">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2743.5</v>
+        <v>2006</v>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
@@ -804,16 +804,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>T126.010.11.013.00</t>
+          <t>T126.010.22.013.01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C11" s="3" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2006</v>
+        <v>2212.5</v>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
@@ -832,16 +832,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>T126.010.22.013.01</t>
+          <t>T126.010.36.013.00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C12" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
@@ -849,7 +849,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2212.5</v>
+        <v>2006</v>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
@@ -860,16 +860,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>T126.010.36.013.00</t>
+          <t>T126.207.11.013.00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C13" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2006</v>
+        <v>3481</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
@@ -888,16 +888,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>T126.207.11.013.00</t>
+          <t>T137.407.11.041.00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C14" s="3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3481</v>
+        <v>3274.5</v>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
@@ -916,12 +916,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T137.407.11.041.00</t>
+          <t>T137.407.11.051.00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C15" s="3" t="n">
@@ -944,16 +944,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T137.407.11.051.00</t>
+          <t>T137.410.11.041.00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SO2311035</t>
+          <t>SO2311043</t>
         </is>
       </c>
       <c r="C16" s="3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
@@ -961,65 +961,9 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3274.5</v>
+        <v>1740.5</v>
       </c>
       <c r="F16" s="3" t="inlineStr">
-        <is>
-          <t>cs</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>T137.410.11.041.00</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SO2311035</t>
-        </is>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>現貨</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>1740.5</v>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>cs</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>T41.1.183.33</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SO2311035</t>
-        </is>
-      </c>
-      <c r="C18" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>現貨</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>2861.5</v>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>cs</t>
         </is>

</xml_diff>